<commit_message>
Finalização da importação das projeções da ESPN, corrigindo os IDs da estatística dos QBs
</commit_message>
<xml_diff>
--- a/static/exports/espn_stat_ids.xlsx
+++ b/static/exports/espn_stat_ids.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gsposito/Projects/DudesFantasyFootball/static/exports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855FD255-7DF3-B34C-9277-90F644D933B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD0A96BA-2259-F942-80C0-9B5ADE7716A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="-2500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="115">
   <si>
     <t>colName</t>
   </si>
@@ -32,15 +32,6 @@
     <t>janName</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
     <t>pass_yds</t>
   </si>
   <si>
@@ -215,72 +206,33 @@
     <t>CAR</t>
   </si>
   <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
     <t>REC</t>
   </si>
   <si>
-    <t>53</t>
-  </si>
-  <si>
-    <t>61</t>
-  </si>
-  <si>
-    <t>51</t>
-  </si>
-  <si>
     <t>Defensive</t>
   </si>
   <si>
-    <t>95</t>
-  </si>
-  <si>
     <t>FR</t>
   </si>
   <si>
-    <t>96</t>
-  </si>
-  <si>
     <t>SCK</t>
   </si>
   <si>
-    <t>99</t>
-  </si>
-  <si>
     <t>TD Return</t>
   </si>
   <si>
     <t>ITD</t>
   </si>
   <si>
-    <t>103</t>
-  </si>
-  <si>
     <t>FTD</t>
   </si>
   <si>
-    <t>104</t>
-  </si>
-  <si>
     <t>FF</t>
   </si>
   <si>
-    <t>106</t>
-  </si>
-  <si>
     <t>TT</t>
   </si>
   <si>
-    <t>109</t>
-  </si>
-  <si>
     <t>appliedTotal</t>
   </si>
   <si>
@@ -294,6 +246,126 @@
   </si>
   <si>
     <t>FPTS</t>
+  </si>
+  <si>
+    <t>fg</t>
+  </si>
+  <si>
+    <t>FG FGM</t>
+  </si>
+  <si>
+    <t>fg_fgm</t>
+  </si>
+  <si>
+    <t>kicking</t>
+  </si>
+  <si>
+    <t>FG39</t>
+  </si>
+  <si>
+    <t>fg_att</t>
+  </si>
+  <si>
+    <t>FG FGA</t>
+  </si>
+  <si>
+    <t>fg_fga</t>
+  </si>
+  <si>
+    <t>FGA39</t>
+  </si>
+  <si>
+    <t>fg_4049</t>
+  </si>
+  <si>
+    <t>FG 40-49</t>
+  </si>
+  <si>
+    <t>fg_40_49</t>
+  </si>
+  <si>
+    <t>FG49</t>
+  </si>
+  <si>
+    <t>fg_50</t>
+  </si>
+  <si>
+    <t>FG 50</t>
+  </si>
+  <si>
+    <t>FG50+</t>
+  </si>
+  <si>
+    <t>fg_att_4049</t>
+  </si>
+  <si>
+    <t>FG 40-49A</t>
+  </si>
+  <si>
+    <t>fg_40_49a</t>
+  </si>
+  <si>
+    <t>FGA49</t>
+  </si>
+  <si>
+    <t>fg_att_50</t>
+  </si>
+  <si>
+    <t>FG 50+A</t>
+  </si>
+  <si>
+    <t>fg_50_a</t>
+  </si>
+  <si>
+    <t>FGA50+</t>
+  </si>
+  <si>
+    <t>xp</t>
+  </si>
+  <si>
+    <t>XP XPM</t>
+  </si>
+  <si>
+    <t>xp_xpm</t>
+  </si>
+  <si>
+    <t>XP</t>
+  </si>
+  <si>
+    <t>xp_att</t>
+  </si>
+  <si>
+    <t>XP XPA</t>
+  </si>
+  <si>
+    <t>xp_xpa</t>
+  </si>
+  <si>
+    <t>XPA</t>
+  </si>
+  <si>
+    <t>pass_comp</t>
+  </si>
+  <si>
+    <t>pass_att</t>
+  </si>
+  <si>
+    <t>PASSING ATT</t>
+  </si>
+  <si>
+    <t>PASSING COMP</t>
+  </si>
+  <si>
+    <t>passing_att</t>
+  </si>
+  <si>
+    <t>passing_comp</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
@@ -645,9 +717,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -667,130 +741,130 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E1" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="F1" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2">
         <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3">
         <v>4</v>
       </c>
       <c r="E3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
+        <v>39</v>
+      </c>
+      <c r="D4">
+        <v>20</v>
       </c>
       <c r="E4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" t="s">
         <v>58</v>
-      </c>
-      <c r="F4" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>108</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>109</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" t="s">
-        <v>64</v>
+        <v>111</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="F5" t="s">
-        <v>63</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>107</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>110</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" t="s">
-        <v>65</v>
+        <v>112</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="F6" t="s">
-        <v>59</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" t="s">
-        <v>66</v>
+        <v>40</v>
+      </c>
+      <c r="D7">
+        <v>23</v>
       </c>
       <c r="E7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F7" t="s">
         <v>60</v>
@@ -798,222 +872,422 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" t="s">
-        <v>68</v>
+        <v>41</v>
+      </c>
+      <c r="D8">
+        <v>24</v>
       </c>
       <c r="E8" t="s">
-        <v>12</v>
+        <v>59</v>
       </c>
       <c r="F8" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>47</v>
-      </c>
-      <c r="D9" t="s">
-        <v>69</v>
+        <v>42</v>
+      </c>
+      <c r="D9">
+        <v>25</v>
       </c>
       <c r="E9" t="s">
-        <v>12</v>
+        <v>59</v>
       </c>
       <c r="F9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" t="s">
-        <v>70</v>
+        <v>43</v>
+      </c>
+      <c r="D10">
+        <v>53</v>
       </c>
       <c r="E10" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F10" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D11" t="s">
-        <v>85</v>
+        <v>44</v>
+      </c>
+      <c r="D11">
+        <v>42</v>
       </c>
       <c r="E11" t="s">
-        <v>71</v>
+        <v>9</v>
       </c>
       <c r="F11" t="s">
-        <v>84</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" t="s">
-        <v>76</v>
+        <v>45</v>
+      </c>
+      <c r="D12">
+        <v>43</v>
       </c>
       <c r="E12" t="s">
-        <v>71</v>
+        <v>9</v>
       </c>
       <c r="F12" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D13" t="s">
-        <v>83</v>
+        <v>46</v>
+      </c>
+      <c r="D13">
+        <v>109</v>
       </c>
       <c r="E13" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="F13" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>52</v>
-      </c>
-      <c r="D14" t="s">
-        <v>74</v>
+        <v>47</v>
+      </c>
+      <c r="D14">
+        <v>99</v>
       </c>
       <c r="E14" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="F14" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s">
-        <v>53</v>
-      </c>
-      <c r="D15" t="s">
-        <v>72</v>
+        <v>48</v>
+      </c>
+      <c r="D15">
+        <v>106</v>
       </c>
       <c r="E15" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="F15" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C16" t="s">
-        <v>54</v>
-      </c>
-      <c r="D16" t="s">
-        <v>79</v>
+        <v>49</v>
+      </c>
+      <c r="D16">
+        <v>96</v>
       </c>
       <c r="E16" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="F16" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
-      </c>
-      <c r="D17" t="s">
-        <v>81</v>
+        <v>50</v>
+      </c>
+      <c r="D17">
+        <v>95</v>
       </c>
       <c r="E17" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="F17" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C18" t="s">
-        <v>56</v>
-      </c>
-      <c r="D18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18">
+        <v>103</v>
+      </c>
+      <c r="E18" t="s">
+        <v>65</v>
+      </c>
+      <c r="F18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19">
+        <v>104</v>
+      </c>
+      <c r="E19" t="s">
+        <v>65</v>
+      </c>
+      <c r="F19" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" t="s">
+        <v>70</v>
+      </c>
+      <c r="E20" t="s">
+        <v>73</v>
+      </c>
+      <c r="F20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>75</v>
+      </c>
+      <c r="B21" t="s">
+        <v>76</v>
+      </c>
+      <c r="C21" t="s">
+        <v>77</v>
+      </c>
+      <c r="D21">
+        <v>80</v>
+      </c>
+      <c r="E21" t="s">
+        <v>78</v>
+      </c>
+      <c r="F21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" t="s">
+        <v>81</v>
+      </c>
+      <c r="C22" t="s">
+        <v>82</v>
+      </c>
+      <c r="D22">
+        <v>81</v>
+      </c>
+      <c r="E22" t="s">
+        <v>78</v>
+      </c>
+      <c r="F22" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>84</v>
+      </c>
+      <c r="B23" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" t="s">
         <v>86</v>
       </c>
-      <c r="E18" t="s">
+      <c r="D23">
+        <v>77</v>
+      </c>
+      <c r="E23" t="s">
+        <v>78</v>
+      </c>
+      <c r="F23" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>88</v>
+      </c>
+      <c r="B24" t="s">
         <v>89</v>
       </c>
-      <c r="F18" t="s">
+      <c r="C24" t="s">
+        <v>88</v>
+      </c>
+      <c r="D24">
+        <v>74</v>
+      </c>
+      <c r="E24" t="s">
+        <v>78</v>
+      </c>
+      <c r="F24" t="s">
         <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>91</v>
+      </c>
+      <c r="B25" t="s">
+        <v>92</v>
+      </c>
+      <c r="C25" t="s">
+        <v>93</v>
+      </c>
+      <c r="D25">
+        <v>78</v>
+      </c>
+      <c r="E25" t="s">
+        <v>78</v>
+      </c>
+      <c r="F25" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>95</v>
+      </c>
+      <c r="B26" t="s">
+        <v>96</v>
+      </c>
+      <c r="C26" t="s">
+        <v>97</v>
+      </c>
+      <c r="D26">
+        <v>75</v>
+      </c>
+      <c r="E26" t="s">
+        <v>78</v>
+      </c>
+      <c r="F26" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>99</v>
+      </c>
+      <c r="B27" t="s">
+        <v>100</v>
+      </c>
+      <c r="C27" t="s">
+        <v>101</v>
+      </c>
+      <c r="D27">
+        <v>86</v>
+      </c>
+      <c r="E27" t="s">
+        <v>78</v>
+      </c>
+      <c r="F27" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>103</v>
+      </c>
+      <c r="B28" t="s">
+        <v>104</v>
+      </c>
+      <c r="C28" t="s">
+        <v>105</v>
+      </c>
+      <c r="D28">
+        <v>87</v>
+      </c>
+      <c r="E28" t="s">
+        <v>78</v>
+      </c>
+      <c r="F28" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>